<commit_message>
Aggiornato allarmi (ma vanno ancora rivisti perche manca l'header del .scl)
</commit_message>
<xml_diff>
--- a/Input/reduced_filtered_AI_hmi_alarms_LibreriaNastri_Master_HmiStructures_R9D.xlsx
+++ b/Input/reduced_filtered_AI_hmi_alarms_LibreriaNastri_Master_HmiStructures_R9D.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stefano.massoletti\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stefano.massoletti.REGROUP\Desktop\LAVORO\Leonardo\_Generiche\Tool Nastri Leonardo\Nastrini-e-Coriandoli\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8FF1002-BFD8-48AA-A3CF-5ADF9EA356D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2BAB5B9-4A0E-4BFC-BD22-1ACFDE9A1851}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-225" windowWidth="29040" windowHeight="15720" tabRatio="1000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="1000" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SV DB" sheetId="18" r:id="rId1"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3752" uniqueCount="1429">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3748" uniqueCount="1426">
   <si>
     <t>0.0</t>
   </si>
@@ -3811,15 +3811,6 @@
     <t>SV_MERGING</t>
   </si>
   <si>
-    <t>SV_DIVERTER</t>
-  </si>
-  <si>
-    <t>SV_BUDDE_LOADER</t>
-  </si>
-  <si>
-    <t>SV_SWIVEL</t>
-  </si>
-  <si>
     <t>SV_CAROUSEL</t>
   </si>
   <si>
@@ -3862,9 +3853,6 @@
     <t>SV_DV10001H</t>
   </si>
   <si>
-    <t>N. DB Commands</t>
-  </si>
-  <si>
     <t xml:space="preserve">CONVEYOR #: Alarms disabled by operator. </t>
   </si>
   <si>
@@ -4340,6 +4328,9 @@
   </si>
   <si>
     <t>SHUTTER #: FAULT condition detected.</t>
+  </si>
+  <si>
+    <t>Word Index</t>
   </si>
 </sst>
 </file>
@@ -4436,7 +4427,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -4452,12 +4443,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4697,9 +4682,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -5010,10 +4997,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection sqref="A1:E1"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5022,10 +5009,9 @@
     <col min="2" max="2" width="22.7109375" customWidth="1"/>
     <col min="3" max="3" width="26" customWidth="1"/>
     <col min="4" max="4" width="23.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
         <v>236</v>
       </c>
@@ -5033,16 +5019,13 @@
         <v>237</v>
       </c>
       <c r="C1" s="26" t="s">
-        <v>1267</v>
-      </c>
-      <c r="D1" s="9" t="s">
-        <v>1269</v>
-      </c>
-      <c r="E1" s="26" t="s">
-        <v>1267</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1264</v>
+      </c>
+      <c r="D1" s="28" t="s">
+        <v>1425</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>1239</v>
       </c>
@@ -5053,13 +5036,10 @@
         <v>20</v>
       </c>
       <c r="D2" s="10">
-        <v>300</v>
-      </c>
-      <c r="E2" s="7">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>1240</v>
       </c>
@@ -5070,13 +5050,10 @@
         <v>48</v>
       </c>
       <c r="D3" s="10">
-        <v>302</v>
-      </c>
-      <c r="E3" s="7">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>1241</v>
       </c>
@@ -5087,13 +5064,10 @@
         <v>11</v>
       </c>
       <c r="D4" s="10">
-        <v>304</v>
-      </c>
-      <c r="E4" s="7">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
         <v>1242</v>
       </c>
@@ -5104,13 +5078,10 @@
         <v>20</v>
       </c>
       <c r="D5" s="10">
-        <v>308</v>
-      </c>
-      <c r="E5" s="7">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>1243</v>
       </c>
@@ -5121,13 +5092,10 @@
         <v>2</v>
       </c>
       <c r="D6" s="10">
-        <v>314</v>
-      </c>
-      <c r="E6" s="7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>1244</v>
       </c>
@@ -5138,13 +5106,10 @@
         <v>36</v>
       </c>
       <c r="D7" s="10">
-        <v>320</v>
-      </c>
-      <c r="E7" s="7">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>1245</v>
       </c>
@@ -5155,13 +5120,10 @@
         <v>190</v>
       </c>
       <c r="D8" s="10">
-        <v>332</v>
-      </c>
-      <c r="E8" s="7">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>1246</v>
       </c>
@@ -5172,13 +5134,10 @@
         <v>104</v>
       </c>
       <c r="D9" s="10">
-        <v>325</v>
-      </c>
-      <c r="E9" s="7">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
         <v>1247</v>
       </c>
@@ -5189,13 +5148,10 @@
         <v>20</v>
       </c>
       <c r="D10" s="10">
-        <v>342</v>
-      </c>
-      <c r="E10" s="7">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
         <v>1248</v>
       </c>
@@ -5206,13 +5162,10 @@
         <v>320</v>
       </c>
       <c r="D11" s="10">
-        <v>350</v>
-      </c>
-      <c r="E11" s="7">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="s">
         <v>1249</v>
       </c>
@@ -5223,13 +5176,10 @@
         <v>10</v>
       </c>
       <c r="D12" s="10">
-        <v>376</v>
-      </c>
-      <c r="E12" s="7">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="13" t="s">
         <v>1250</v>
       </c>
@@ -5240,13 +5190,10 @@
         <v>6</v>
       </c>
       <c r="D13" s="10">
-        <v>386</v>
-      </c>
-      <c r="E13" s="7">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="s">
         <v>1251</v>
       </c>
@@ -5257,113 +5204,61 @@
         <v>22</v>
       </c>
       <c r="D14" s="10">
-        <v>388</v>
-      </c>
-      <c r="E14" s="7">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="27" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="13" t="s">
         <v>1252</v>
       </c>
       <c r="B15" s="10">
-        <v>396</v>
-      </c>
-      <c r="C15" s="7"/>
+        <v>322</v>
+      </c>
+      <c r="C15" s="7">
+        <v>34</v>
+      </c>
       <c r="D15" s="10">
-        <v>396</v>
-      </c>
-      <c r="E15" s="7"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="27" t="s">
-        <v>1253</v>
+        <v>310</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="13" t="s">
+        <v>1265</v>
       </c>
       <c r="B16" s="10">
-        <v>500</v>
+        <v>398</v>
       </c>
       <c r="C16" s="7"/>
       <c r="D16" s="10">
-        <v>500</v>
-      </c>
-      <c r="E16" s="7"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="27" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="13" t="s">
+        <v>1253</v>
+      </c>
+      <c r="B17" s="10">
+        <v>326</v>
+      </c>
+      <c r="C17" s="7">
+        <v>4</v>
+      </c>
+      <c r="D17" s="10">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="14" t="s">
         <v>1254</v>
       </c>
-      <c r="B17" s="10">
-        <v>1501</v>
-      </c>
-      <c r="C17" s="7"/>
-      <c r="D17" s="10">
-        <v>1501</v>
-      </c>
-      <c r="E17" s="7"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="13" t="s">
-        <v>1255</v>
-      </c>
-      <c r="B18" s="10">
-        <v>322</v>
-      </c>
-      <c r="C18" s="7">
-        <v>34</v>
-      </c>
-      <c r="D18" s="10">
-        <v>322</v>
-      </c>
-      <c r="E18" s="7">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="13" t="s">
-        <v>1268</v>
-      </c>
-      <c r="B19" s="10">
-        <v>398</v>
-      </c>
-      <c r="C19" s="7"/>
-      <c r="D19" s="10">
-        <v>398</v>
-      </c>
-      <c r="E19" s="7"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="13" t="s">
-        <v>1256</v>
-      </c>
-      <c r="B20" s="10">
-        <v>326</v>
-      </c>
-      <c r="C20" s="7">
-        <v>4</v>
-      </c>
-      <c r="D20" s="10">
-        <v>326</v>
-      </c>
-      <c r="E20" s="7">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="14" t="s">
-        <v>1257</v>
-      </c>
-      <c r="B21" s="11">
+      <c r="B18" s="11">
         <v>306</v>
       </c>
-      <c r="C21" s="8">
-        <v>2</v>
-      </c>
-      <c r="D21" s="11">
-        <v>306</v>
-      </c>
-      <c r="E21" s="8">
-        <v>2</v>
+      <c r="C18" s="8">
+        <v>2</v>
+      </c>
+      <c r="D18" s="11">
+        <v>340</v>
       </c>
     </row>
   </sheetData>
@@ -5404,7 +5299,7 @@
         <v>526</v>
       </c>
       <c r="E1" t="s">
-        <v>1258</v>
+        <v>1255</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -5697,7 +5592,7 @@
         <v>984</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>1264</v>
+        <v>1261</v>
       </c>
       <c r="E21" s="6"/>
     </row>
@@ -5998,7 +5893,7 @@
         <v>761</v>
       </c>
       <c r="E41" s="6" t="s">
-        <v>1315</v>
+        <v>1311</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
@@ -6015,7 +5910,7 @@
         <v>762</v>
       </c>
       <c r="E42" s="6" t="s">
-        <v>1314</v>
+        <v>1310</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
@@ -6138,7 +6033,7 @@
         <v>764</v>
       </c>
       <c r="E51" s="6" t="s">
-        <v>1316</v>
+        <v>1312</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
@@ -6155,7 +6050,7 @@
         <v>765</v>
       </c>
       <c r="E52" s="6" t="s">
-        <v>1317</v>
+        <v>1313</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
@@ -6172,7 +6067,7 @@
         <v>766</v>
       </c>
       <c r="E53" s="6" t="s">
-        <v>1318</v>
+        <v>1314</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
@@ -6189,7 +6084,7 @@
         <v>767</v>
       </c>
       <c r="E54" s="6" t="s">
-        <v>1319</v>
+        <v>1315</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
@@ -6206,7 +6101,7 @@
         <v>768</v>
       </c>
       <c r="E55" s="6" t="s">
-        <v>1320</v>
+        <v>1316</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
@@ -6221,7 +6116,7 @@
       </c>
       <c r="D56" s="2"/>
       <c r="E56" s="6" t="s">
-        <v>1321</v>
+        <v>1317</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
@@ -6238,7 +6133,7 @@
         <v>1057</v>
       </c>
       <c r="E57" s="6" t="s">
-        <v>1322</v>
+        <v>1318</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
@@ -6255,7 +6150,7 @@
         <v>1058</v>
       </c>
       <c r="E58" s="6" t="s">
-        <v>1323</v>
+        <v>1319</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
@@ -6272,7 +6167,7 @@
         <v>769</v>
       </c>
       <c r="E59" s="6" t="s">
-        <v>1324</v>
+        <v>1320</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
@@ -6289,7 +6184,7 @@
         <v>770</v>
       </c>
       <c r="E60" s="6" t="s">
-        <v>1325</v>
+        <v>1321</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
@@ -6306,7 +6201,7 @@
         <v>771</v>
       </c>
       <c r="E61" s="6" t="s">
-        <v>1326</v>
+        <v>1322</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
@@ -6323,7 +6218,7 @@
         <v>772</v>
       </c>
       <c r="E62" s="6" t="s">
-        <v>1327</v>
+        <v>1323</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
@@ -6340,7 +6235,7 @@
         <v>773</v>
       </c>
       <c r="E63" s="6" t="s">
-        <v>1328</v>
+        <v>1324</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
@@ -6355,7 +6250,7 @@
       </c>
       <c r="D64" s="2"/>
       <c r="E64" s="6" t="s">
-        <v>1329</v>
+        <v>1325</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
@@ -6370,7 +6265,7 @@
       </c>
       <c r="D65" s="2"/>
       <c r="E65" s="6" t="s">
-        <v>1330</v>
+        <v>1326</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
@@ -6385,7 +6280,7 @@
       </c>
       <c r="D66" s="2"/>
       <c r="E66" s="6" t="s">
-        <v>1331</v>
+        <v>1327</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
@@ -6400,7 +6295,7 @@
       </c>
       <c r="D67" s="2"/>
       <c r="E67" s="6" t="s">
-        <v>1332</v>
+        <v>1328</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
@@ -6415,7 +6310,7 @@
       </c>
       <c r="D68" s="2"/>
       <c r="E68" s="6" t="s">
-        <v>1333</v>
+        <v>1329</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
@@ -6430,7 +6325,7 @@
       </c>
       <c r="D69" s="2"/>
       <c r="E69" s="6" t="s">
-        <v>1334</v>
+        <v>1330</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
@@ -6445,7 +6340,7 @@
       </c>
       <c r="D70" s="2"/>
       <c r="E70" s="6" t="s">
-        <v>1335</v>
+        <v>1331</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
@@ -6551,7 +6446,7 @@
       </c>
       <c r="D78" s="2"/>
       <c r="E78" s="6" t="s">
-        <v>1259</v>
+        <v>1256</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
@@ -6566,7 +6461,7 @@
       </c>
       <c r="D79" s="2"/>
       <c r="E79" s="6" t="s">
-        <v>1260</v>
+        <v>1257</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
@@ -6607,7 +6502,7 @@
       </c>
       <c r="D82" s="2"/>
       <c r="E82" s="6" t="s">
-        <v>1261</v>
+        <v>1258</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
@@ -6635,7 +6530,7 @@
       </c>
       <c r="D84" s="2"/>
       <c r="E84" s="6" t="s">
-        <v>1262</v>
+        <v>1259</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
@@ -6676,7 +6571,7 @@
       </c>
       <c r="D87" s="2"/>
       <c r="E87" s="6" t="s">
-        <v>1265</v>
+        <v>1262</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
@@ -7574,7 +7469,7 @@
         <v>526</v>
       </c>
       <c r="E1" s="19" t="s">
-        <v>1258</v>
+        <v>1255</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -7886,7 +7781,7 @@
         <v>255</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>1336</v>
+        <v>1332</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -8369,7 +8264,7 @@
         <v>278</v>
       </c>
       <c r="E58" s="6" t="s">
-        <v>1337</v>
+        <v>1333</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
@@ -8386,7 +8281,7 @@
         <v>279</v>
       </c>
       <c r="E59" s="6" t="s">
-        <v>1338</v>
+        <v>1334</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
@@ -8403,7 +8298,7 @@
         <v>280</v>
       </c>
       <c r="E60" s="6" t="s">
-        <v>1339</v>
+        <v>1335</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
@@ -8420,7 +8315,7 @@
         <v>281</v>
       </c>
       <c r="E61" s="6" t="s">
-        <v>1340</v>
+        <v>1336</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
@@ -8437,7 +8332,7 @@
         <v>282</v>
       </c>
       <c r="E62" s="6" t="s">
-        <v>1341</v>
+        <v>1337</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
@@ -8454,7 +8349,7 @@
         <v>248</v>
       </c>
       <c r="E63" s="6" t="s">
-        <v>1342</v>
+        <v>1338</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
@@ -8471,7 +8366,7 @@
         <v>286</v>
       </c>
       <c r="E64" s="6" t="s">
-        <v>1343</v>
+        <v>1339</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
@@ -8788,7 +8683,7 @@
         <v>526</v>
       </c>
       <c r="E1" s="19" t="s">
-        <v>1258</v>
+        <v>1255</v>
       </c>
       <c r="F1" s="6"/>
       <c r="G1" s="6"/>
@@ -8950,7 +8845,7 @@
         <v>783</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>1344</v>
+        <v>1340</v>
       </c>
       <c r="F11" s="6"/>
       <c r="G11" s="6"/>
@@ -8969,7 +8864,7 @@
         <v>785</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>1345</v>
+        <v>1341</v>
       </c>
       <c r="F12" s="6"/>
       <c r="G12" s="6"/>
@@ -8988,7 +8883,7 @@
         <v>787</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>1346</v>
+        <v>1342</v>
       </c>
       <c r="F13" s="6"/>
       <c r="G13" s="6"/>
@@ -9007,7 +8902,7 @@
         <v>789</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>1347</v>
+        <v>1343</v>
       </c>
       <c r="F14" s="6"/>
       <c r="G14" s="6"/>
@@ -9220,7 +9115,7 @@
         <v>526</v>
       </c>
       <c r="E1" s="19" t="s">
-        <v>1258</v>
+        <v>1255</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -9305,7 +9200,7 @@
         <v>805</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>1348</v>
+        <v>1344</v>
       </c>
       <c r="G6" s="6"/>
       <c r="H6" s="6"/>
@@ -9324,7 +9219,7 @@
         <v>807</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>1349</v>
+        <v>1345</v>
       </c>
       <c r="G7" s="6"/>
       <c r="H7" s="6"/>
@@ -9343,7 +9238,7 @@
         <v>809</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>1350</v>
+        <v>1346</v>
       </c>
       <c r="G8" s="6"/>
       <c r="H8" s="6"/>
@@ -9362,7 +9257,7 @@
         <v>811</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>1351</v>
+        <v>1347</v>
       </c>
       <c r="G9" s="6"/>
       <c r="H9" s="6"/>
@@ -9381,7 +9276,7 @@
         <v>813</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>1352</v>
+        <v>1348</v>
       </c>
       <c r="G10" s="6"/>
       <c r="H10" s="6"/>
@@ -9400,7 +9295,7 @@
         <v>815</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>1353</v>
+        <v>1349</v>
       </c>
       <c r="G11" s="6"/>
       <c r="H11" s="6"/>
@@ -9491,7 +9386,7 @@
         <v>526</v>
       </c>
       <c r="E1" s="19" t="s">
-        <v>1258</v>
+        <v>1255</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -9566,7 +9461,7 @@
         <v>823</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>1354</v>
+        <v>1350</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -9751,7 +9646,7 @@
         <v>830</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>1355</v>
+        <v>1351</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -9768,7 +9663,7 @@
         <v>831</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>1356</v>
+        <v>1352</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -9785,7 +9680,7 @@
         <v>832</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>1357</v>
+        <v>1353</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -9802,7 +9697,7 @@
         <v>833</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>1358</v>
+        <v>1354</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -9819,7 +9714,7 @@
         <v>834</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>1359</v>
+        <v>1355</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -9834,7 +9729,7 @@
       </c>
       <c r="D24" s="2"/>
       <c r="E24" s="6" t="s">
-        <v>1360</v>
+        <v>1356</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -9921,7 +9816,7 @@
         <v>526</v>
       </c>
       <c r="E1" s="19" t="s">
-        <v>1258</v>
+        <v>1255</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -10101,7 +9996,7 @@
       </c>
       <c r="D13" s="22"/>
       <c r="E13" s="6" t="s">
-        <v>1361</v>
+        <v>1357</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -10424,7 +10319,7 @@
         <v>1226</v>
       </c>
       <c r="E37" s="6" t="s">
-        <v>1362</v>
+        <v>1358</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
@@ -10441,7 +10336,7 @@
         <v>1044</v>
       </c>
       <c r="E38" s="6" t="s">
-        <v>1363</v>
+        <v>1359</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
@@ -10458,7 +10353,7 @@
         <v>1216</v>
       </c>
       <c r="E39" s="6" t="s">
-        <v>1364</v>
+        <v>1360</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
@@ -10475,7 +10370,7 @@
         <v>1217</v>
       </c>
       <c r="E40" s="6" t="s">
-        <v>1365</v>
+        <v>1361</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
@@ -10492,7 +10387,7 @@
         <v>1218</v>
       </c>
       <c r="E41" s="6" t="s">
-        <v>1366</v>
+        <v>1362</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
@@ -10509,7 +10404,7 @@
         <v>1219</v>
       </c>
       <c r="E42" s="6" t="s">
-        <v>1367</v>
+        <v>1363</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
@@ -10526,7 +10421,7 @@
         <v>1220</v>
       </c>
       <c r="E43" s="6" t="s">
-        <v>1368</v>
+        <v>1364</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
@@ -10543,7 +10438,7 @@
         <v>1221</v>
       </c>
       <c r="E44" s="6" t="s">
-        <v>1369</v>
+        <v>1365</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
@@ -10560,7 +10455,7 @@
         <v>1222</v>
       </c>
       <c r="E45" s="6" t="s">
-        <v>1370</v>
+        <v>1366</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
@@ -10577,7 +10472,7 @@
         <v>1223</v>
       </c>
       <c r="E46" s="6" t="s">
-        <v>1371</v>
+        <v>1367</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
@@ -10594,7 +10489,7 @@
         <v>1224</v>
       </c>
       <c r="E47" s="6" t="s">
-        <v>1372</v>
+        <v>1368</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
@@ -10611,7 +10506,7 @@
         <v>1225</v>
       </c>
       <c r="E48" s="6" t="s">
-        <v>1373</v>
+        <v>1369</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
@@ -10628,7 +10523,7 @@
         <v>1045</v>
       </c>
       <c r="E49" s="6" t="s">
-        <v>1374</v>
+        <v>1370</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
@@ -10645,7 +10540,7 @@
         <v>1046</v>
       </c>
       <c r="E50" s="6" t="s">
-        <v>1375</v>
+        <v>1371</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
@@ -10662,7 +10557,7 @@
         <v>1211</v>
       </c>
       <c r="E51" s="6" t="s">
-        <v>1376</v>
+        <v>1372</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
@@ -10679,7 +10574,7 @@
         <v>1212</v>
       </c>
       <c r="E52" s="6" t="s">
-        <v>1377</v>
+        <v>1373</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
@@ -10696,7 +10591,7 @@
         <v>1215</v>
       </c>
       <c r="E53" s="6" t="s">
-        <v>1378</v>
+        <v>1374</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
@@ -10713,7 +10608,7 @@
         <v>1047</v>
       </c>
       <c r="E54" s="6" t="s">
-        <v>1379</v>
+        <v>1375</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
@@ -10730,7 +10625,7 @@
         <v>1048</v>
       </c>
       <c r="E55" s="6" t="s">
-        <v>1380</v>
+        <v>1376</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
@@ -10747,7 +10642,7 @@
         <v>1049</v>
       </c>
       <c r="E56" s="6" t="s">
-        <v>1381</v>
+        <v>1377</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
@@ -10764,7 +10659,7 @@
         <v>1050</v>
       </c>
       <c r="E57" s="6" t="s">
-        <v>1382</v>
+        <v>1378</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
@@ -10781,7 +10676,7 @@
         <v>1051</v>
       </c>
       <c r="E58" s="6" t="s">
-        <v>1383</v>
+        <v>1379</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
@@ -10798,7 +10693,7 @@
         <v>1052</v>
       </c>
       <c r="E59" s="6" t="s">
-        <v>1384</v>
+        <v>1380</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
@@ -10815,7 +10710,7 @@
         <v>1053</v>
       </c>
       <c r="E60" s="6" t="s">
-        <v>1385</v>
+        <v>1381</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
@@ -10832,7 +10727,7 @@
         <v>1054</v>
       </c>
       <c r="E61" s="6" t="s">
-        <v>1386</v>
+        <v>1382</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
@@ -10849,7 +10744,7 @@
         <v>1055</v>
       </c>
       <c r="E62" s="6" t="s">
-        <v>1387</v>
+        <v>1383</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
@@ -10866,7 +10761,7 @@
         <v>1056</v>
       </c>
       <c r="E63" s="6" t="s">
-        <v>1388</v>
+        <v>1384</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
@@ -10883,7 +10778,7 @@
         <v>1213</v>
       </c>
       <c r="E64" s="6" t="s">
-        <v>1389</v>
+        <v>1385</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
@@ -10900,7 +10795,7 @@
         <v>1214</v>
       </c>
       <c r="E65" s="6" t="s">
-        <v>1390</v>
+        <v>1386</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
@@ -11075,7 +10970,7 @@
         <v>526</v>
       </c>
       <c r="E1" s="19" t="s">
-        <v>1258</v>
+        <v>1255</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -11401,7 +11296,7 @@
         <v>255</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>1391</v>
+        <v>1387</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -11800,7 +11695,7 @@
         <v>273</v>
       </c>
       <c r="E50" s="6" t="s">
-        <v>1396</v>
+        <v>1392</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
@@ -11817,7 +11712,7 @@
         <v>274</v>
       </c>
       <c r="E51" s="6" t="s">
-        <v>1397</v>
+        <v>1393</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
@@ -11834,7 +11729,7 @@
         <v>275</v>
       </c>
       <c r="E52" s="6" t="s">
-        <v>1398</v>
+        <v>1394</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
@@ -11851,7 +11746,7 @@
         <v>276</v>
       </c>
       <c r="E53" s="6" t="s">
-        <v>1399</v>
+        <v>1395</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
@@ -11868,7 +11763,7 @@
         <v>277</v>
       </c>
       <c r="E54" s="6" t="s">
-        <v>1400</v>
+        <v>1396</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
@@ -11885,7 +11780,7 @@
         <v>248</v>
       </c>
       <c r="E55" s="6" t="s">
-        <v>1401</v>
+        <v>1397</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
@@ -11902,7 +11797,7 @@
         <v>879</v>
       </c>
       <c r="E56" s="6" t="s">
-        <v>1402</v>
+        <v>1398</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
@@ -11947,7 +11842,7 @@
         <v>279</v>
       </c>
       <c r="E59" s="6" t="s">
-        <v>1392</v>
+        <v>1388</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
@@ -11964,7 +11859,7 @@
         <v>280</v>
       </c>
       <c r="E60" s="6" t="s">
-        <v>1393</v>
+        <v>1389</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
@@ -11981,7 +11876,7 @@
         <v>281</v>
       </c>
       <c r="E61" s="6" t="s">
-        <v>1394</v>
+        <v>1390</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
@@ -11998,7 +11893,7 @@
         <v>282</v>
       </c>
       <c r="E62" s="6" t="s">
-        <v>1395</v>
+        <v>1391</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
@@ -12333,7 +12228,7 @@
         <v>526</v>
       </c>
       <c r="E1" s="18" t="s">
-        <v>1258</v>
+        <v>1255</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -13008,7 +12903,7 @@
         <v>273</v>
       </c>
       <c r="E50" s="6" t="s">
-        <v>1408</v>
+        <v>1404</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
@@ -13025,7 +12920,7 @@
         <v>274</v>
       </c>
       <c r="E51" s="6" t="s">
-        <v>1409</v>
+        <v>1405</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
@@ -13042,7 +12937,7 @@
         <v>275</v>
       </c>
       <c r="E52" s="6" t="s">
-        <v>1410</v>
+        <v>1406</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
@@ -13059,7 +12954,7 @@
         <v>276</v>
       </c>
       <c r="E53" s="6" t="s">
-        <v>1411</v>
+        <v>1407</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
@@ -13076,7 +12971,7 @@
         <v>277</v>
       </c>
       <c r="E54" s="6" t="s">
-        <v>1412</v>
+        <v>1408</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
@@ -13093,7 +12988,7 @@
         <v>248</v>
       </c>
       <c r="E55" s="6" t="s">
-        <v>1413</v>
+        <v>1409</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
@@ -13136,7 +13031,7 @@
         <v>278</v>
       </c>
       <c r="E58" s="6" t="s">
-        <v>1403</v>
+        <v>1399</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
@@ -13153,7 +13048,7 @@
         <v>279</v>
       </c>
       <c r="E59" s="6" t="s">
-        <v>1404</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
@@ -13248,7 +13143,7 @@
         <v>889</v>
       </c>
       <c r="E66" s="6" t="s">
-        <v>1405</v>
+        <v>1401</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
@@ -13265,7 +13160,7 @@
         <v>891</v>
       </c>
       <c r="E67" s="6" t="s">
-        <v>1406</v>
+        <v>1402</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
@@ -13282,7 +13177,7 @@
         <v>893</v>
       </c>
       <c r="E68" s="6" t="s">
-        <v>1407</v>
+        <v>1403</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
@@ -13539,7 +13434,7 @@
         <v>526</v>
       </c>
       <c r="E1" s="19" t="s">
-        <v>1258</v>
+        <v>1255</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -13778,7 +13673,7 @@
         <v>1204</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>1266</v>
+        <v>1263</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -13795,7 +13690,7 @@
         <v>1206</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>1414</v>
+        <v>1410</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -14024,7 +13919,7 @@
         <v>526</v>
       </c>
       <c r="E1" s="19" t="s">
-        <v>1258</v>
+        <v>1255</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -14158,7 +14053,7 @@
         <v>1117</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>1415</v>
+        <v>1411</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -14175,7 +14070,7 @@
         <v>1118</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>1416</v>
+        <v>1412</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -14192,7 +14087,7 @@
         <v>1119</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>1417</v>
+        <v>1413</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -14483,7 +14378,7 @@
         <v>526</v>
       </c>
       <c r="E1" s="19" t="s">
-        <v>1258</v>
+        <v>1255</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -14513,7 +14408,7 @@
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="6" t="s">
-        <v>1300</v>
+        <v>1296</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -14718,7 +14613,7 @@
         <v>529</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>1293</v>
+        <v>1289</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -14735,7 +14630,7 @@
         <v>530</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>1294</v>
+        <v>1290</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -14752,7 +14647,7 @@
         <v>684</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>1295</v>
+        <v>1291</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -14769,7 +14664,7 @@
         <v>531</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>1296</v>
+        <v>1292</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -14786,7 +14681,7 @@
         <v>532</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>1297</v>
+        <v>1293</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -14803,7 +14698,7 @@
         <v>533</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>1298</v>
+        <v>1294</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -14820,7 +14715,7 @@
         <v>534</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>1299</v>
+        <v>1295</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -16920,7 +16815,7 @@
         <v>526</v>
       </c>
       <c r="E1" s="19" t="s">
-        <v>1258</v>
+        <v>1255</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -16967,7 +16862,7 @@
         <v>1198</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>1428</v>
+        <v>1424</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -17199,7 +17094,7 @@
         <v>526</v>
       </c>
       <c r="E1" s="19" t="s">
-        <v>1258</v>
+        <v>1255</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -17555,8 +17450,8 @@
       <c r="D26" s="2" t="s">
         <v>700</v>
       </c>
-      <c r="E26" s="28" t="s">
-        <v>1301</v>
+      <c r="E26" s="27" t="s">
+        <v>1297</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -17572,8 +17467,8 @@
       <c r="D27" s="2" t="s">
         <v>701</v>
       </c>
-      <c r="E27" s="28" t="s">
-        <v>1302</v>
+      <c r="E27" s="27" t="s">
+        <v>1298</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -17589,8 +17484,8 @@
       <c r="D28" s="2" t="s">
         <v>702</v>
       </c>
-      <c r="E28" s="28" t="s">
-        <v>1303</v>
+      <c r="E28" s="27" t="s">
+        <v>1299</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -17606,8 +17501,8 @@
       <c r="D29" s="2" t="s">
         <v>703</v>
       </c>
-      <c r="E29" s="28" t="s">
-        <v>1304</v>
+      <c r="E29" s="27" t="s">
+        <v>1300</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -18055,8 +17950,8 @@
   </sheetPr>
   <dimension ref="A1:E35"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E35"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18084,7 +17979,7 @@
         <v>526</v>
       </c>
       <c r="E1" s="19" t="s">
-        <v>1258</v>
+        <v>1255</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -18220,8 +18115,8 @@
       <c r="D10" s="2" t="s">
         <v>246</v>
       </c>
-      <c r="E10" s="28" t="s">
-        <v>1305</v>
+      <c r="E10" s="27" t="s">
+        <v>1301</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -18237,8 +18132,8 @@
       <c r="D11" s="2" t="s">
         <v>247</v>
       </c>
-      <c r="E11" s="28" t="s">
-        <v>1306</v>
+      <c r="E11" s="27" t="s">
+        <v>1302</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -18254,8 +18149,8 @@
       <c r="D12" s="2" t="s">
         <v>248</v>
       </c>
-      <c r="E12" s="28" t="s">
-        <v>1307</v>
+      <c r="E12" s="27" t="s">
+        <v>1303</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -18271,8 +18166,8 @@
       <c r="D13" s="2" t="s">
         <v>249</v>
       </c>
-      <c r="E13" s="28" t="s">
-        <v>1308</v>
+      <c r="E13" s="27" t="s">
+        <v>1304</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -18288,7 +18183,7 @@
       <c r="D14" s="2" t="s">
         <v>250</v>
       </c>
-      <c r="E14" s="6"/>
+      <c r="E14" s="27"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="16">
@@ -18303,7 +18198,7 @@
       <c r="D15" s="2" t="s">
         <v>251</v>
       </c>
-      <c r="E15" s="6"/>
+      <c r="E15" s="27"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="16">
@@ -18316,7 +18211,7 @@
         <v>2</v>
       </c>
       <c r="D16" s="2"/>
-      <c r="E16" s="6"/>
+      <c r="E16" s="27"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="16">
@@ -18329,7 +18224,7 @@
         <v>2</v>
       </c>
       <c r="D17" s="2"/>
-      <c r="E17" s="6"/>
+      <c r="E17" s="27"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="16">
@@ -18342,7 +18237,7 @@
         <v>2</v>
       </c>
       <c r="D18" s="2"/>
-      <c r="E18" s="6"/>
+      <c r="E18" s="27"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="16">
@@ -18355,7 +18250,7 @@
         <v>2</v>
       </c>
       <c r="D19" s="2"/>
-      <c r="E19" s="6"/>
+      <c r="E19" s="27"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="16">
@@ -18368,7 +18263,7 @@
         <v>2</v>
       </c>
       <c r="D20" s="2"/>
-      <c r="E20" s="6"/>
+      <c r="E20" s="27"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="16">
@@ -18381,7 +18276,7 @@
         <v>2</v>
       </c>
       <c r="D21" s="2"/>
-      <c r="E21" s="6"/>
+      <c r="E21" s="27"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="16">
@@ -18394,7 +18289,7 @@
         <v>2</v>
       </c>
       <c r="D22" s="2"/>
-      <c r="E22" s="6"/>
+      <c r="E22" s="27"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="16">
@@ -18407,7 +18302,7 @@
         <v>925</v>
       </c>
       <c r="D23" s="2"/>
-      <c r="E23" s="6"/>
+      <c r="E23" s="27"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="16">
@@ -18420,7 +18315,7 @@
         <v>2</v>
       </c>
       <c r="D24" s="2"/>
-      <c r="E24" s="6"/>
+      <c r="E24" s="27"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="16">
@@ -18433,7 +18328,7 @@
         <v>2</v>
       </c>
       <c r="D25" s="2"/>
-      <c r="E25" s="6"/>
+      <c r="E25" s="27"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="16">
@@ -18606,7 +18501,7 @@
         <v>526</v>
       </c>
       <c r="E1" s="19" t="s">
-        <v>1258</v>
+        <v>1255</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -18638,7 +18533,7 @@
         <v>711</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>1263</v>
+        <v>1260</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -18847,7 +18742,7 @@
         <v>717</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>1309</v>
+        <v>1305</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -19092,7 +18987,7 @@
         <v>526</v>
       </c>
       <c r="E1" s="19" t="s">
-        <v>1258</v>
+        <v>1255</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -19199,7 +19094,7 @@
         <v>271</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>1310</v>
+        <v>1306</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -19335,8 +19230,8 @@
   </sheetPr>
   <dimension ref="A1:E87"/>
   <sheetViews>
-    <sheetView topLeftCell="A82" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E124" sqref="E124"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19364,7 +19259,7 @@
         <v>526</v>
       </c>
       <c r="E1" s="19" t="s">
-        <v>1258</v>
+        <v>1255</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -19780,7 +19675,7 @@
         <v>260</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>1270</v>
+        <v>1266</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -19960,7 +19855,7 @@
         <v>271</v>
       </c>
       <c r="E41" s="6" t="s">
-        <v>1271</v>
+        <v>1267</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
@@ -19977,7 +19872,7 @@
         <v>272</v>
       </c>
       <c r="E42" s="6" t="s">
-        <v>1272</v>
+        <v>1268</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
@@ -20085,7 +19980,7 @@
         <v>273</v>
       </c>
       <c r="E50" s="6" t="s">
-        <v>1273</v>
+        <v>1269</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
@@ -20102,7 +19997,7 @@
         <v>274</v>
       </c>
       <c r="E51" s="6" t="s">
-        <v>1274</v>
+        <v>1270</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
@@ -20119,7 +20014,7 @@
         <v>275</v>
       </c>
       <c r="E52" s="6" t="s">
-        <v>1275</v>
+        <v>1271</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
@@ -20136,7 +20031,7 @@
         <v>276</v>
       </c>
       <c r="E53" s="6" t="s">
-        <v>1276</v>
+        <v>1272</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
@@ -20153,7 +20048,7 @@
         <v>277</v>
       </c>
       <c r="E54" s="6" t="s">
-        <v>1277</v>
+        <v>1273</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
@@ -20170,7 +20065,7 @@
         <v>248</v>
       </c>
       <c r="E55" s="6" t="s">
-        <v>1278</v>
+        <v>1274</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
@@ -20185,7 +20080,7 @@
       </c>
       <c r="D56" s="2"/>
       <c r="E56" s="6" t="s">
-        <v>1279</v>
+        <v>1275</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
@@ -20200,7 +20095,7 @@
       </c>
       <c r="D57" s="2"/>
       <c r="E57" s="6" t="s">
-        <v>1280</v>
+        <v>1276</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
@@ -20217,7 +20112,7 @@
         <v>278</v>
       </c>
       <c r="E58" s="6" t="s">
-        <v>1286</v>
+        <v>1282</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
@@ -20234,7 +20129,7 @@
         <v>279</v>
       </c>
       <c r="E59" s="6" t="s">
-        <v>1287</v>
+        <v>1283</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
@@ -20251,7 +20146,7 @@
         <v>280</v>
       </c>
       <c r="E60" s="6" t="s">
-        <v>1288</v>
+        <v>1284</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
@@ -20268,7 +20163,7 @@
         <v>281</v>
       </c>
       <c r="E61" s="6" t="s">
-        <v>1289</v>
+        <v>1285</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
@@ -20285,7 +20180,7 @@
         <v>282</v>
       </c>
       <c r="E62" s="6" t="s">
-        <v>1290</v>
+        <v>1286</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
@@ -20300,7 +20195,7 @@
       </c>
       <c r="D63" s="2"/>
       <c r="E63" s="6" t="s">
-        <v>1291</v>
+        <v>1287</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
@@ -20315,7 +20210,7 @@
       </c>
       <c r="D64" s="2"/>
       <c r="E64" s="6" t="s">
-        <v>1292</v>
+        <v>1288</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
@@ -20427,7 +20322,7 @@
       </c>
       <c r="D72" s="2"/>
       <c r="E72" s="6" t="s">
-        <v>1281</v>
+        <v>1277</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
@@ -20442,7 +20337,7 @@
       </c>
       <c r="D73" s="2"/>
       <c r="E73" s="6" t="s">
-        <v>1282</v>
+        <v>1278</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
@@ -20483,7 +20378,7 @@
       </c>
       <c r="D76" s="2"/>
       <c r="E76" s="6" t="s">
-        <v>1283</v>
+        <v>1279</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
@@ -20498,7 +20393,7 @@
       </c>
       <c r="D77" s="2"/>
       <c r="E77" s="6" t="s">
-        <v>1284</v>
+        <v>1280</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
@@ -20513,7 +20408,7 @@
       </c>
       <c r="D78" s="2"/>
       <c r="E78" s="6" t="s">
-        <v>1285</v>
+        <v>1281</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
@@ -20669,7 +20564,7 @@
         <v>526</v>
       </c>
       <c r="E1" s="19" t="s">
-        <v>1258</v>
+        <v>1255</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -21396,7 +21291,7 @@
         <v>274</v>
       </c>
       <c r="E50" s="6" t="s">
-        <v>1418</v>
+        <v>1414</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
@@ -21413,7 +21308,7 @@
         <v>274</v>
       </c>
       <c r="E51" s="6" t="s">
-        <v>1419</v>
+        <v>1415</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
@@ -21430,7 +21325,7 @@
         <v>275</v>
       </c>
       <c r="E52" s="6" t="s">
-        <v>1420</v>
+        <v>1416</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
@@ -21447,7 +21342,7 @@
         <v>275</v>
       </c>
       <c r="E53" s="6" t="s">
-        <v>1421</v>
+        <v>1417</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
@@ -21464,7 +21359,7 @@
         <v>276</v>
       </c>
       <c r="E54" s="6" t="s">
-        <v>1422</v>
+        <v>1418</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
@@ -21481,7 +21376,7 @@
         <v>277</v>
       </c>
       <c r="E55" s="6" t="s">
-        <v>1423</v>
+        <v>1419</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
@@ -21498,7 +21393,7 @@
         <v>248</v>
       </c>
       <c r="E56" s="6" t="s">
-        <v>1424</v>
+        <v>1420</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
@@ -21515,7 +21410,7 @@
         <v>1180</v>
       </c>
       <c r="E57" s="6" t="s">
-        <v>1425</v>
+        <v>1421</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
@@ -21532,7 +21427,7 @@
         <v>1181</v>
       </c>
       <c r="E58" s="6" t="s">
-        <v>1426</v>
+        <v>1422</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
@@ -21549,7 +21444,7 @@
         <v>1167</v>
       </c>
       <c r="E59" s="6" t="s">
-        <v>1427</v>
+        <v>1423</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
@@ -21978,7 +21873,7 @@
         <v>526</v>
       </c>
       <c r="E1" s="19" t="s">
-        <v>1258</v>
+        <v>1255</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -22038,7 +21933,7 @@
         <v>720</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>1311</v>
+        <v>1307</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -22055,7 +21950,7 @@
         <v>721</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>1312</v>
+        <v>1308</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -22072,7 +21967,7 @@
         <v>722</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>1313</v>
+        <v>1309</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -24064,7 +23959,22 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6F42FBFE-7A75-46D3-8582-FF1095977D3C}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6F42FBFE-7A75-46D3-8582-FF1095977D3C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="383b0bb7-e620-4e20-ae9e-4f262a20ab07"/>
+    <ds:schemaRef ds:uri="aca03388-b78c-4415-a826-d0bf4eb594c5"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -24081,6 +23991,7 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="383b0bb7-e620-4e20-ae9e-4f262a20ab07"/>
+    <ds:schemaRef ds:uri="aca03388-b78c-4415-a826-d0bf4eb594c5"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>